<commit_message>
Add an alternative material for DS38W
</commit_message>
<xml_diff>
--- a/2_Release/Light-Box V1.00.00/Light-Box-B001/Light-Box-B001_BOM_V1.00.00.xlsx
+++ b/2_Release/Light-Box V1.00.00/Light-Box-B001/Light-Box-B001_BOM_V1.00.00.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541D5867-A9B8-4159-BC13-5B6956D8EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF48AB-981B-4090-A2F3-A50CB8A8D20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="295">
   <si>
     <t xml:space="preserve">Bill of Materials </t>
   </si>
@@ -953,13 +953,17 @@
   </si>
   <si>
     <t>C17888</t>
+  </si>
+  <si>
+    <t>DSK34</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,8 +999,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1012,6 +1023,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1061,6 +1078,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1400,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1881,7 +1899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1914,7 +1932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1947,7 +1965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1980,7 +1998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2013,7 +2031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2046,7 +2064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2079,7 +2097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2112,7 +2130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2144,8 +2162,11 @@
       <c r="J25" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2178,7 +2199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2211,7 +2232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2244,7 +2265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2277,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2310,7 +2331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2343,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>26</v>

</xml_diff>